<commit_message>
Timesheet update en presentatie
</commit_message>
<xml_diff>
--- a/doc/Timesheet_Lee_Van_Hecke.xlsx
+++ b/doc/Timesheet_Lee_Van_Hecke.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Datum</t>
   </si>
@@ -73,6 +73,9 @@
     <t>Alle beschikbare bleutooth aparaten detecteren &amp; en connectie maken met 1</t>
   </si>
   <si>
+    <t>Research / development</t>
+  </si>
+  <si>
     <t>Onderzoeken authentication met JWT</t>
   </si>
   <si>
@@ -83,6 +86,33 @@
   </si>
   <si>
     <t>Authentication clientside</t>
+  </si>
+  <si>
+    <t>Integrating passport (auth)</t>
+  </si>
+  <si>
+    <t>Onderzoeken Redux</t>
+  </si>
+  <si>
+    <t>API users</t>
+  </si>
+  <si>
+    <t>Files opkuisen</t>
+  </si>
+  <si>
+    <t>Redux</t>
+  </si>
+  <si>
+    <t>Roles voor docenten te tonen</t>
+  </si>
+  <si>
+    <t>bekijken ble plugin</t>
+  </si>
+  <si>
+    <t>auth in orde brengen</t>
+  </si>
+  <si>
+    <t>Presentatie, files opkuisen &amp; afwerken waar mogelijk</t>
   </si>
 </sst>
 </file>
@@ -271,7 +301,7 @@
       </c>
       <c r="G3" s="9">
         <f>SUM(D2:D77)</f>
-        <v>50.5</v>
+        <v>94.5</v>
       </c>
     </row>
     <row r="4" ht="22.5" customHeight="1">
@@ -432,11 +462,11 @@
       <c r="A15" s="12">
         <v>43081.0</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>14</v>
+      <c r="B15" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" s="13">
         <v>2.0</v>
@@ -450,7 +480,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" s="16">
         <v>3.25</v>
@@ -464,7 +494,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" s="13">
         <v>2.0</v>
@@ -478,65 +508,137 @@
         <v>14</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D18" s="16">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="19" ht="22.5" customHeight="1">
+      <c r="A19" s="12">
+        <v>43089.0</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="13">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="20" ht="22.5" customHeight="1">
+      <c r="A20" s="15">
+        <v>43091.0</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="16">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="21" ht="22.5" customHeight="1">
+      <c r="A21" s="12">
+        <v>43097.0</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="13">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="22" ht="22.5" customHeight="1">
+      <c r="A22" s="15">
+        <v>43104.0</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="16">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="23" ht="22.5" customHeight="1">
+      <c r="A23" s="12">
+        <v>43105.0</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="13">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="24" ht="22.5" customHeight="1">
+      <c r="A24" s="15">
+        <v>43108.0</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="16">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="25" ht="22.5" customHeight="1">
+      <c r="A25" s="12">
+        <v>43109.0</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="13">
         <v>6.0</v>
       </c>
     </row>
-    <row r="19" ht="22.5" customHeight="1">
-      <c r="A19" s="5"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="18"/>
-    </row>
-    <row r="20" ht="22.5" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" ht="22.5" customHeight="1">
-      <c r="A21" s="5"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="18"/>
-    </row>
-    <row r="22" ht="22.5" customHeight="1">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" ht="22.5" customHeight="1">
-      <c r="A23" s="5"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="18"/>
-    </row>
-    <row r="24" ht="22.5" customHeight="1">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" ht="22.5" customHeight="1">
-      <c r="A25" s="5"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="18"/>
-    </row>
     <row r="26" ht="22.5" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="3"/>
+      <c r="A26" s="15">
+        <v>43110.0</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="16">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="27" ht="22.5" customHeight="1">
-      <c r="A27" s="5"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="18"/>
+      <c r="A27" s="12">
+        <v>43111.0</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="13">
+        <v>10.0</v>
+      </c>
     </row>
     <row r="28" ht="22.5" customHeight="1">
       <c r="A28" s="3"/>

</xml_diff>